<commit_message>
Tweaked footprints for wire terminals; fixed up some mechanical issues on output board (incl. removing resistor networks)
</commit_message>
<xml_diff>
--- a/output_board-bom.xlsx
+++ b/output_board-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5A2F33-B8A9-044A-BBBE-022B868F96C8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22047CF2-D6B2-0543-B4DD-AD18AC19FA29}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lichtenstein_onion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="92">
   <si>
     <t>Part</t>
   </si>
@@ -136,18 +136,6 @@
     <t>517-30310-6002</t>
   </si>
   <si>
-    <t>RN1</t>
-  </si>
-  <si>
-    <t>RN2</t>
-  </si>
-  <si>
-    <t>Chip Resistor Array 4 Single Resistor</t>
-  </si>
-  <si>
-    <t>CTS742C083</t>
-  </si>
-  <si>
     <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/output_board.sch at 20180530 2138</t>
   </si>
   <si>
@@ -205,9 +193,6 @@
     <t>652-CR0805JW-361ELF</t>
   </si>
   <si>
-    <t>71-CRA04S0803102JRT7</t>
-  </si>
-  <si>
     <t>PCB terminal block - PTS 1,5/ 8-5,0-H - 1792928</t>
   </si>
   <si>
@@ -226,12 +211,6 @@
     <t>SV5</t>
   </si>
   <si>
-    <t>﻿571-1-2199298-4</t>
-  </si>
-  <si>
-    <t>﻿571-1-2199298-5</t>
-  </si>
-  <si>
     <t>16-pin DIP socket</t>
   </si>
   <si>
@@ -242,6 +221,81 @@
   </si>
   <si>
     <t>604-APTR3216YC</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R-EU_M0806</t>
+  </si>
+  <si>
+    <t>M0806</t>
+  </si>
+  <si>
+    <t>R-EU_M0807</t>
+  </si>
+  <si>
+    <t>M0807</t>
+  </si>
+  <si>
+    <t>R-EU_M0808</t>
+  </si>
+  <si>
+    <t>M0808</t>
+  </si>
+  <si>
+    <t>R-EU_M0809</t>
+  </si>
+  <si>
+    <t>M0809</t>
+  </si>
+  <si>
+    <t>R-EU_M0810</t>
+  </si>
+  <si>
+    <t>M0810</t>
+  </si>
+  <si>
+    <t>R-EU_M0811</t>
+  </si>
+  <si>
+    <t>M0811</t>
+  </si>
+  <si>
+    <t>R-EU_M0812</t>
+  </si>
+  <si>
+    <t>M0812</t>
+  </si>
+  <si>
+    <t>R-EU_M0813</t>
+  </si>
+  <si>
+    <t>M0813</t>
+  </si>
+  <si>
+    <t>571-1-2199298-4</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1151,7 +1205,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1205,61 +1259,61 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G7" s="6"/>
     </row>
@@ -1268,19 +1322,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G8" s="6"/>
     </row>
@@ -1289,19 +1343,19 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" s="6"/>
     </row>
@@ -1320,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G10" s="6"/>
     </row>
@@ -1329,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -1341,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G11" s="6"/>
     </row>
@@ -1350,7 +1404,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
@@ -1362,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="6"/>
     </row>
@@ -1371,7 +1425,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -1383,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G13" s="6"/>
     </row>
@@ -1392,7 +1446,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
@@ -1404,7 +1458,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -1413,7 +1467,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -1425,7 +1479,7 @@
         <v>23</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G15" s="6"/>
     </row>
@@ -1434,7 +1488,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>21</v>
@@ -1446,7 +1500,7 @@
         <v>23</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G16" s="6"/>
     </row>
@@ -1455,7 +1509,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>21</v>
@@ -1467,7 +1521,7 @@
         <v>23</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G17" s="6"/>
     </row>
@@ -1476,7 +1530,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
@@ -1488,7 +1542,7 @@
         <v>23</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G18" s="6"/>
     </row>
@@ -1497,7 +1551,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
@@ -1509,221 +1563,277 @@
         <v>23</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1792928</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1792928</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1792928</v>
+        <v>69</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1792863</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1792863</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1792863</v>
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1792928</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1792928</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1792928</v>
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1792928</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1792928</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1792928</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1792863</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1792863</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1792863</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="8"/>
+      <c r="A30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1792928</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1792928</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1792928</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="4"/>
+      <c r="A31" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="8"/>
+      <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="4"/>
+      <c r="A32" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="8"/>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7">
@@ -1736,21 +1846,37 @@
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="4"/>
+      <c r="A34" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="8"/>
+      <c r="D34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="4"/>
+      <c r="A35" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="8"/>
+      <c r="D35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7">
@@ -1870,29 +1996,83 @@
       <c r="F48" s="8"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="11"/>
-      <c r="B49" s="12"/>
+    <row r="49" spans="1:7">
+      <c r="A49" s="4"/>
+      <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="4"/>
+      <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="10"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="4"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="4"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="4"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="4"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="11"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="11"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
corrected output board bom
</commit_message>
<xml_diff>
--- a/output_board-bom.xlsx
+++ b/output_board-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22047CF2-D6B2-0543-B4DD-AD18AC19FA29}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665EEAFD-2EE8-304E-89C6-9CFDF99AF719}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lichtenstein_onion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
   <si>
     <t>Part</t>
   </si>
@@ -245,54 +245,6 @@
   </si>
   <si>
     <t>R17</t>
-  </si>
-  <si>
-    <t>R-EU_M0806</t>
-  </si>
-  <si>
-    <t>M0806</t>
-  </si>
-  <si>
-    <t>R-EU_M0807</t>
-  </si>
-  <si>
-    <t>M0807</t>
-  </si>
-  <si>
-    <t>R-EU_M0808</t>
-  </si>
-  <si>
-    <t>M0808</t>
-  </si>
-  <si>
-    <t>R-EU_M0809</t>
-  </si>
-  <si>
-    <t>M0809</t>
-  </si>
-  <si>
-    <t>R-EU_M0810</t>
-  </si>
-  <si>
-    <t>M0810</t>
-  </si>
-  <si>
-    <t>R-EU_M0811</t>
-  </si>
-  <si>
-    <t>M0811</t>
-  </si>
-  <si>
-    <t>R-EU_M0812</t>
-  </si>
-  <si>
-    <t>M0812</t>
-  </si>
-  <si>
-    <t>R-EU_M0813</t>
-  </si>
-  <si>
-    <t>M0813</t>
   </si>
   <si>
     <t>571-1-2199298-4</t>
@@ -1190,7 +1142,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1575,10 +1527,10 @@
         <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
@@ -1596,10 +1548,10 @@
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>23</v>
@@ -1617,10 +1569,10 @@
         <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>23</v>
@@ -1638,10 +1590,10 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>23</v>
@@ -1659,10 +1611,10 @@
         <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>23</v>
@@ -1680,10 +1632,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>23</v>
@@ -1701,10 +1653,10 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>23</v>
@@ -1722,10 +1674,10 @@
         <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>23</v>
@@ -1858,7 +1810,7 @@
         <v>63</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G34" s="6"/>
     </row>
@@ -1875,7 +1827,7 @@
         <v>63</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G35" s="6"/>
     </row>

</xml_diff>

<commit_message>
Minor revisions to output board
</commit_message>
<xml_diff>
--- a/output_board-bom.xlsx
+++ b/output_board-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665EEAFD-2EE8-304E-89C6-9CFDF99AF719}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F659BD-F8A4-1643-A890-38F92BCC180E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1335,7 +1335,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -1347,7 +1347,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G11" s="6"/>
     </row>

</xml_diff>